<commit_message>
# added support for overexpressions
</commit_message>
<xml_diff>
--- a/PredictionFiles/Supplemental Excel File 6- CSD Template.xlsx
+++ b/PredictionFiles/Supplemental Excel File 6- CSD Template.xlsx
@@ -10671,14 +10671,14 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C14" s="4"/>
-      <c r="D14" s="0" t="s">
+      <c r="D14" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F14" s="4"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C15" s="4"/>
-      <c r="E15" s="0" t="s">
+      <c r="E15" s="1" t="s">
         <v>9</v>
       </c>
       <c r="F15" s="4"/>
@@ -10766,21 +10766,21 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D21" activeCellId="0" sqref="D21"/>
+      <selection pane="topLeft" activeCell="D27" activeCellId="0" sqref="D27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>22</v>
       </c>
     </row>
@@ -11326,471 +11326,354 @@
     </row>
     <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="1"/>
-      <c r="B119" s="0"/>
     </row>
     <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="1"/>
-      <c r="B120" s="0"/>
     </row>
     <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="1"/>
-      <c r="B121" s="0"/>
     </row>
     <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="1"/>
-      <c r="B122" s="0"/>
     </row>
     <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="1"/>
-      <c r="B123" s="0"/>
     </row>
     <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="1"/>
-      <c r="B124" s="0"/>
     </row>
     <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="1"/>
-      <c r="B125" s="0"/>
     </row>
     <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="1"/>
-      <c r="B126" s="0"/>
     </row>
     <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="1"/>
-      <c r="B127" s="0"/>
     </row>
     <row r="128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="1"/>
-      <c r="B128" s="0"/>
     </row>
     <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="1"/>
-      <c r="B129" s="0"/>
     </row>
     <row r="130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="1"/>
-      <c r="B130" s="0"/>
     </row>
     <row r="131" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="1"/>
-      <c r="B131" s="0"/>
     </row>
     <row r="132" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="1"/>
-      <c r="B132" s="0"/>
     </row>
     <row r="133" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="1"/>
-      <c r="B133" s="0"/>
     </row>
     <row r="134" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="1"/>
-      <c r="B134" s="0"/>
     </row>
     <row r="135" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="1"/>
-      <c r="B135" s="0"/>
     </row>
     <row r="136" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="1"/>
-      <c r="B136" s="0"/>
     </row>
     <row r="137" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="1"/>
-      <c r="B137" s="0"/>
     </row>
     <row r="138" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="1"/>
-      <c r="B138" s="0"/>
     </row>
     <row r="139" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="1"/>
-      <c r="B139" s="0"/>
     </row>
     <row r="140" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="1"/>
-      <c r="B140" s="0"/>
     </row>
     <row r="141" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="1"/>
-      <c r="B141" s="0"/>
     </row>
     <row r="142" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="1"/>
-      <c r="B142" s="0"/>
     </row>
     <row r="143" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="1"/>
-      <c r="B143" s="0"/>
     </row>
     <row r="144" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="1"/>
-      <c r="B144" s="0"/>
     </row>
     <row r="145" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="1"/>
-      <c r="B145" s="0"/>
     </row>
     <row r="146" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="1"/>
-      <c r="B146" s="0"/>
     </row>
     <row r="147" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="1"/>
-      <c r="B147" s="0"/>
     </row>
     <row r="148" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="1"/>
-      <c r="B148" s="0"/>
     </row>
     <row r="149" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="1"/>
-      <c r="B149" s="0"/>
     </row>
     <row r="150" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="1"/>
-      <c r="B150" s="0"/>
     </row>
     <row r="151" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="1"/>
-      <c r="B151" s="0"/>
     </row>
     <row r="152" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="1"/>
-      <c r="B152" s="0"/>
     </row>
     <row r="153" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="1"/>
-      <c r="B153" s="0"/>
     </row>
     <row r="154" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="1"/>
-      <c r="B154" s="0"/>
     </row>
     <row r="155" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="1"/>
-      <c r="B155" s="0"/>
     </row>
     <row r="156" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="1"/>
-      <c r="B156" s="0"/>
     </row>
     <row r="157" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="1"/>
-      <c r="B157" s="0"/>
     </row>
     <row r="158" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="1"/>
-      <c r="B158" s="0"/>
     </row>
     <row r="159" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="1"/>
-      <c r="B159" s="0"/>
     </row>
     <row r="160" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="1"/>
-      <c r="B160" s="0"/>
     </row>
     <row r="161" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="1"/>
-      <c r="B161" s="0"/>
     </row>
     <row r="162" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="1"/>
-      <c r="B162" s="0"/>
     </row>
     <row r="163" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="1"/>
-      <c r="B163" s="0"/>
     </row>
     <row r="164" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="1"/>
-      <c r="B164" s="0"/>
     </row>
     <row r="165" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="1"/>
-      <c r="B165" s="0"/>
     </row>
     <row r="166" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="1"/>
-      <c r="B166" s="0"/>
     </row>
     <row r="167" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="1"/>
-      <c r="B167" s="0"/>
     </row>
     <row r="168" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="1"/>
-      <c r="B168" s="0"/>
     </row>
     <row r="169" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="1"/>
-      <c r="B169" s="0"/>
     </row>
     <row r="170" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="1"/>
-      <c r="B170" s="0"/>
     </row>
     <row r="171" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="1"/>
-      <c r="B171" s="0"/>
     </row>
     <row r="172" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="1"/>
-      <c r="B172" s="0"/>
     </row>
     <row r="173" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="1"/>
-      <c r="B173" s="0"/>
     </row>
     <row r="174" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="1"/>
-      <c r="B174" s="0"/>
     </row>
     <row r="175" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="1"/>
-      <c r="B175" s="0"/>
     </row>
     <row r="176" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="1"/>
-      <c r="B176" s="0"/>
     </row>
     <row r="177" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="1"/>
-      <c r="B177" s="0"/>
     </row>
     <row r="178" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="1"/>
-      <c r="B178" s="0"/>
     </row>
     <row r="179" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="1"/>
-      <c r="B179" s="0"/>
     </row>
     <row r="180" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="1"/>
-      <c r="B180" s="0"/>
     </row>
     <row r="181" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="1"/>
-      <c r="B181" s="0"/>
     </row>
     <row r="182" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="1"/>
-      <c r="B182" s="0"/>
     </row>
     <row r="183" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="1"/>
-      <c r="B183" s="0"/>
     </row>
     <row r="184" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="1"/>
-      <c r="B184" s="0"/>
     </row>
     <row r="185" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="1"/>
-      <c r="B185" s="0"/>
     </row>
     <row r="186" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="1"/>
-      <c r="B186" s="0"/>
     </row>
     <row r="187" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="1"/>
-      <c r="B187" s="0"/>
     </row>
     <row r="188" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="1"/>
-      <c r="B188" s="0"/>
     </row>
     <row r="189" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="1"/>
-      <c r="B189" s="0"/>
     </row>
     <row r="190" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="1"/>
-      <c r="B190" s="0"/>
     </row>
     <row r="191" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="1"/>
-      <c r="B191" s="0"/>
     </row>
     <row r="192" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A192" s="1"/>
-      <c r="B192" s="0"/>
     </row>
     <row r="193" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A193" s="1"/>
-      <c r="B193" s="0"/>
     </row>
     <row r="194" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A194" s="1"/>
-      <c r="B194" s="0"/>
     </row>
     <row r="195" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A195" s="1"/>
-      <c r="B195" s="0"/>
     </row>
     <row r="196" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="1"/>
-      <c r="B196" s="0"/>
     </row>
     <row r="197" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="1"/>
-      <c r="B197" s="0"/>
     </row>
     <row r="198" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="1"/>
-      <c r="B198" s="0"/>
     </row>
     <row r="199" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="1"/>
-      <c r="B199" s="0"/>
     </row>
     <row r="200" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="1"/>
-      <c r="B200" s="0"/>
     </row>
     <row r="201" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="1"/>
-      <c r="B201" s="0"/>
     </row>
     <row r="202" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A202" s="1"/>
-      <c r="B202" s="0"/>
     </row>
     <row r="203" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A203" s="1"/>
-      <c r="B203" s="0"/>
     </row>
     <row r="204" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A204" s="1"/>
-      <c r="B204" s="0"/>
     </row>
     <row r="205" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="1"/>
-      <c r="B205" s="0"/>
     </row>
     <row r="206" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A206" s="1"/>
-      <c r="B206" s="0"/>
     </row>
     <row r="207" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A207" s="1"/>
-      <c r="B207" s="0"/>
     </row>
     <row r="208" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A208" s="1"/>
-      <c r="B208" s="0"/>
     </row>
     <row r="209" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A209" s="1"/>
-      <c r="B209" s="0"/>
     </row>
     <row r="210" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A210" s="1"/>
-      <c r="B210" s="0"/>
     </row>
     <row r="211" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A211" s="1"/>
-      <c r="B211" s="0"/>
     </row>
     <row r="212" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A212" s="1"/>
-      <c r="B212" s="0"/>
     </row>
     <row r="213" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A213" s="1"/>
-      <c r="B213" s="0"/>
     </row>
     <row r="214" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A214" s="1"/>
-      <c r="B214" s="0"/>
     </row>
     <row r="215" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A215" s="1"/>
-      <c r="B215" s="0"/>
     </row>
     <row r="216" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A216" s="1"/>
-      <c r="B216" s="0"/>
     </row>
     <row r="217" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A217" s="1"/>
-      <c r="B217" s="0"/>
     </row>
     <row r="218" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A218" s="1"/>
-      <c r="B218" s="0"/>
     </row>
     <row r="219" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A219" s="1"/>
-      <c r="B219" s="0"/>
     </row>
     <row r="220" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A220" s="1"/>
-      <c r="B220" s="0"/>
     </row>
     <row r="221" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A221" s="1"/>
-      <c r="B221" s="0"/>
     </row>
     <row r="222" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A222" s="1"/>
-      <c r="B222" s="0"/>
     </row>
     <row r="223" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A223" s="1"/>
-      <c r="B223" s="0"/>
     </row>
     <row r="224" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A224" s="1"/>
-      <c r="B224" s="0"/>
     </row>
     <row r="225" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A225" s="1"/>
-      <c r="B225" s="0"/>
     </row>
     <row r="226" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A226" s="1"/>
-      <c r="B226" s="0"/>
     </row>
     <row r="227" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A227" s="1"/>
-      <c r="B227" s="0"/>
     </row>
     <row r="228" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A228" s="1"/>
-      <c r="B228" s="0"/>
     </row>
     <row r="229" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A229" s="1"/>
-      <c r="B229" s="0"/>
     </row>
     <row r="230" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A230" s="1"/>
-      <c r="B230" s="0"/>
     </row>
     <row r="231" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A231" s="1"/>
-      <c r="B231" s="0"/>
     </row>
     <row r="232" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A232" s="1"/>
-      <c r="B232" s="0"/>
     </row>
     <row r="233" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A233" s="1"/>
-      <c r="B233" s="0"/>
     </row>
     <row r="234" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A234" s="1"/>
-      <c r="B234" s="0"/>
     </row>
     <row r="235" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A235" s="1"/>
-      <c r="B235" s="0"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>